<commit_message>
add more to assembly
- orings
- module pcb
- improve bom
</commit_message>
<xml_diff>
--- a/case/signpost_case_bom.xlsx
+++ b/case/signpost_case_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Part</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>#1177N11</t>
+  </si>
+  <si>
+    <t>8-32x5/8 flat</t>
+  </si>
+  <si>
+    <t>4-40x1/8</t>
+  </si>
+  <si>
+    <t>4-40x5/16</t>
+  </si>
+  <si>
+    <t>4-40x3/8 torx</t>
   </si>
 </sst>
 </file>
@@ -406,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,15 +429,16 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="52.375" customWidth="1"/>
     <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="87.875" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -474,6 +487,9 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -485,6 +501,9 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -496,6 +515,9 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -506,6 +528,9 @@
       </c>
       <c r="D7" t="s">
         <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed black oxide parts to zinc allow
</commit_message>
<xml_diff>
--- a/case/signpost_case_bom.xlsx
+++ b/case/signpost_case_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Solar panel mount screws</t>
   </si>
   <si>
-    <t xml:space="preserve">91251A106</t>
+    <t xml:space="preserve">90128A106</t>
   </si>
   <si>
     <t xml:space="preserve">4-40 x ¼ Socket head cap</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Signpost attachment Bolts</t>
   </si>
   <si>
-    <t xml:space="preserve">90044A149</t>
+    <t xml:space="preserve">90128A636</t>
   </si>
   <si>
     <t xml:space="preserve">3/8-16 x 3 socket head cap</t>
@@ -256,18 +256,18 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.9023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.693023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.693023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added standoff for backplane
</commit_message>
<xml_diff>
--- a/case/signpost_case_bom.xlsx
+++ b/case/signpost_case_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t xml:space="preserve">1177N11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module standoffs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91780A531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module standoff screws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90272A106</t>
   </si>
 </sst>
 </file>
@@ -253,21 +265,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.693023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.693023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.0604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,6 +485,28 @@
       </c>
       <c r="D14" s="0" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>